<commit_message>
Updated Meta and added Tempus AI
</commit_message>
<xml_diff>
--- a/ACMR vs Naura.xlsx
+++ b/ACMR vs Naura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerem\OneDrive\Masaüstü\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A3FDEC5-F5CF-4444-BDC3-076D57122A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66C89AB-788F-4132-81D5-DD4731178D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5028" yWindow="744" windowWidth="32424" windowHeight="14424" xr2:uid="{B960F72B-CB41-486A-96EB-54BBD62D27A5}"/>
+    <workbookView xWindow="30696" yWindow="612" windowWidth="27216" windowHeight="16008" xr2:uid="{B960F72B-CB41-486A-96EB-54BBD62D27A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -262,18 +262,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="39" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="39" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -882,6 +881,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1149272799"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2761,15 +2761,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>125504</xdr:colOff>
+      <xdr:colOff>537881</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>143435</xdr:rowOff>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>690281</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>367552</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>107576</xdr:rowOff>
+      <xdr:rowOff>98612</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3322,8 +3322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37726EE8-C020-4FB2-8852-EE15E5341288}">
   <dimension ref="B2:X13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.69921875" defaultRowHeight="16.95" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3396,641 +3396,634 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>42.186</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>104.395</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>133.709</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>108.542</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>74.256</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>144.577</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>168.56899999999999</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>170.321</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>152.191</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="5">
         <v>202.48</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="5">
         <v>203.976</v>
       </c>
-      <c r="O3" s="6">
+      <c r="O3" s="5">
         <v>223.471</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="5">
         <v>172.34700000000001</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="5">
         <v>215.37200000000001</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="5">
         <v>269.16000000000003</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S3" s="5">
         <v>248.41800000000001</v>
       </c>
-      <c r="T3" s="6">
+      <c r="T3" s="5">
         <v>215.38200000000001</v>
       </c>
-      <c r="U3" s="6">
+      <c r="U3" s="5">
         <v>259.077</v>
       </c>
-      <c r="V3" s="6">
+      <c r="V3" s="5">
         <v>293.02100000000002</v>
       </c>
-      <c r="W3" s="7">
+      <c r="W3" s="6">
         <v>284.92500000000001</v>
       </c>
     </row>
     <row r="4" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10">
+      <c r="D4" s="8"/>
+      <c r="E4" s="9">
         <f>(E3-D3)/D3</f>
         <v>1.4746361352107333</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <f t="shared" ref="F4:W4" si="0">(F3-E3)/E3</f>
         <v>0.28079888883567228</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="9">
         <f t="shared" si="0"/>
         <v>-0.1882221839965896</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <f t="shared" si="0"/>
         <v>-0.315877724751709</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <f t="shared" si="0"/>
         <v>0.94700764921353153</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <f t="shared" si="0"/>
         <v>0.16594617401108053</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <f t="shared" si="0"/>
         <v>1.03933700739757E-2</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="9">
         <f t="shared" si="0"/>
         <v>-0.10644606360930241</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <f t="shared" si="0"/>
         <v>0.33043346847054023</v>
       </c>
-      <c r="N4" s="10">
+      <c r="N4" s="9">
         <f t="shared" si="0"/>
         <v>7.3883840379297188E-3</v>
       </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <f t="shared" si="0"/>
         <v>9.5574969604267188E-2</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="9">
         <f t="shared" si="0"/>
         <v>-0.22877241342277072</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="9">
         <f t="shared" si="0"/>
         <v>0.24964171119891848</v>
       </c>
-      <c r="R4" s="10">
+      <c r="R4" s="9">
         <f t="shared" si="0"/>
         <v>0.24974462789963417</v>
       </c>
-      <c r="S4" s="10">
+      <c r="S4" s="9">
         <f t="shared" si="0"/>
         <v>-7.7061970575122665E-2</v>
       </c>
-      <c r="T4" s="10">
+      <c r="T4" s="9">
         <f t="shared" si="0"/>
         <v>-0.13298553244933942</v>
       </c>
-      <c r="U4" s="10">
+      <c r="U4" s="9">
         <f t="shared" si="0"/>
         <v>0.20287210630414795</v>
       </c>
-      <c r="V4" s="10">
+      <c r="V4" s="9">
         <f t="shared" si="0"/>
         <v>0.13101896347417955</v>
       </c>
-      <c r="W4" s="11">
+      <c r="W4" s="10">
         <f t="shared" si="0"/>
         <v>-2.7629419051876838E-2</v>
       </c>
     </row>
     <row r="5" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>-5.7859999999999996</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>12.236000000000001</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>21.004000000000001</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>11.808999999999999</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>7.1449999999999996</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>26.824999999999999</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>25.678999999999998</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>17.7</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>34.597000000000001</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>24.21</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="5">
         <v>42.372</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <v>31.08</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>20.38</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>29.76</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="5">
         <v>35.889000000000003</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="5">
         <v>29.616700000000002</v>
       </c>
-      <c r="T5" s="6">
+      <c r="T5" s="5">
         <v>22.893799999999999</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="5">
         <v>32.104399999999998</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="5">
         <v>38.255200000000002</v>
       </c>
-      <c r="W5" s="7">
+      <c r="W5" s="6">
         <v>38.837200000000003</v>
       </c>
     </row>
     <row r="6" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14">
+      <c r="C6" s="12"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13">
         <f t="shared" ref="F6" si="1">(F5-E5)/E5</f>
         <v>0.7165740438051651</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <f t="shared" ref="G6" si="2">(G5-F5)/F5</f>
         <v>-0.43777375737954682</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <f t="shared" ref="H6" si="3">(H5-G5)/G5</f>
         <v>-0.39495300194766703</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
         <f t="shared" ref="I6" si="4">(I5-H5)/H5</f>
         <v>2.754373687893632</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <f t="shared" ref="J6" si="5">(J5-I5)/I5</f>
         <v>-4.2721342031686892E-2</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <f t="shared" ref="K6" si="6">(K5-J5)/J5</f>
         <v>-0.31072082246193389</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <f t="shared" ref="L6" si="7">(L5-K5)/K5</f>
         <v>0.95463276836158206</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="13">
         <f t="shared" ref="M6" si="8">(M5-L5)/L5</f>
         <v>-0.30022834349799116</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="13">
         <f t="shared" ref="N6" si="9">(N5-M5)/M5</f>
         <v>0.75018587360594791</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="13">
         <f t="shared" ref="O6" si="10">(O5-N5)/N5</f>
         <v>-0.26649674313225719</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="13">
         <f t="shared" ref="P6" si="11">(P5-O5)/O5</f>
         <v>-0.34427284427284427</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="Q6" s="13">
         <f t="shared" ref="Q6" si="12">(Q5-P5)/P5</f>
         <v>0.4602551521099118</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6" s="13">
         <f t="shared" ref="R6" si="13">(R5-Q5)/Q5</f>
         <v>0.20594758064516133</v>
       </c>
-      <c r="S6" s="14">
+      <c r="S6" s="13">
         <f t="shared" ref="S6" si="14">(S5-R5)/R5</f>
         <v>-0.1747694279584274</v>
       </c>
-      <c r="T6" s="14">
+      <c r="T6" s="13">
         <f t="shared" ref="T6" si="15">(T5-S5)/S5</f>
         <v>-0.22699693078567168</v>
       </c>
-      <c r="U6" s="14">
+      <c r="U6" s="13">
         <f t="shared" ref="U6" si="16">(U5-T5)/T5</f>
         <v>0.40231853165485854</v>
       </c>
-      <c r="V6" s="14">
+      <c r="V6" s="13">
         <f t="shared" ref="V6" si="17">(V5-U5)/U5</f>
         <v>0.19158744595756358</v>
       </c>
-      <c r="W6" s="15">
+      <c r="W6" s="14">
         <f t="shared" ref="W6" si="18">(W5-V5)/V5</f>
         <v>1.5213618017942677E-2</v>
       </c>
     </row>
     <row r="7" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>323.03899999999999</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>479.44099999999997</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>625.87300000000005</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>674.923</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>558.73099999999999</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>624.66099999999994</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>842.02200000000005</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>1034.45</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>808.51700000000005</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="5">
         <v>908.71500000000003</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="5">
         <v>1125.6400000000001</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="5">
         <v>1302.18</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="5">
         <v>1124.23</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <v>1112.6099999999999</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="5">
         <v>1568.87</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="5">
         <v>1728.04</v>
       </c>
-      <c r="T7" s="6">
+      <c r="T7" s="5">
         <v>1487.41</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U7" s="5">
         <v>1668.91</v>
       </c>
-      <c r="V7" s="6">
+      <c r="V7" s="5">
         <v>1909.63</v>
       </c>
-      <c r="W7" s="7">
+      <c r="W7" s="6">
         <v>2078.31</v>
       </c>
     </row>
     <row r="8" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <f>(E7-D7)/D7</f>
         <v>0.48415825952903518</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <f t="shared" ref="F8" si="19">(F7-E7)/E7</f>
         <v>0.30542235645261895</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="9">
         <f t="shared" ref="G8" si="20">(G7-F7)/F7</f>
         <v>7.8370532040845264E-2</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="9">
         <f t="shared" ref="H8" si="21">(H7-G7)/G7</f>
         <v>-0.17215593482515784</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <f t="shared" ref="I8" si="22">(I7-H7)/H7</f>
         <v>0.11799953823933154</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <f t="shared" ref="J8" si="23">(J7-I7)/I7</f>
         <v>0.34796633694115708</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="9">
         <f t="shared" ref="K8" si="24">(K7-J7)/J7</f>
         <v>0.22853084598739698</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="9">
         <f t="shared" ref="L8" si="25">(L7-K7)/K7</f>
         <v>-0.21840881627918216</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="9">
         <f t="shared" ref="M8" si="26">(M7-L7)/L7</f>
         <v>0.12392813014444962</v>
       </c>
-      <c r="N8" s="10">
+      <c r="N8" s="9">
         <f t="shared" ref="N8" si="27">(N7-M7)/M7</f>
         <v>0.23871620915248462</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <f t="shared" ref="O8" si="28">(O7-N7)/N7</f>
         <v>0.1568352226289044</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="9">
         <f t="shared" ref="P8" si="29">(P7-O7)/O7</f>
         <v>-0.13665545469904317</v>
       </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="9">
         <f t="shared" ref="Q8" si="30">(Q7-P7)/P7</f>
         <v>-1.0335963281535023E-2</v>
       </c>
-      <c r="R8" s="10">
+      <c r="R8" s="9">
         <f t="shared" ref="R8" si="31">(R7-Q7)/Q7</f>
         <v>0.41008080099945177</v>
       </c>
-      <c r="S8" s="10">
+      <c r="S8" s="9">
         <f t="shared" ref="S8" si="32">(S7-R7)/R7</f>
         <v>0.10145518749163417</v>
       </c>
-      <c r="T8" s="10">
+      <c r="T8" s="9">
         <f t="shared" ref="T8" si="33">(T7-S7)/S7</f>
         <v>-0.1392502488368324</v>
       </c>
-      <c r="U8" s="10">
+      <c r="U8" s="9">
         <f t="shared" ref="U8" si="34">(U7-T7)/T7</f>
         <v>0.12202418969887253</v>
       </c>
-      <c r="V8" s="10">
+      <c r="V8" s="9">
         <f t="shared" ref="V8" si="35">(V7-U7)/U7</f>
         <v>0.14423785584603124</v>
       </c>
-      <c r="W8" s="11">
+      <c r="W8" s="10">
         <f t="shared" ref="W8" si="36">(W7-V7)/V7</f>
         <v>8.83312474144205E-2</v>
       </c>
     </row>
     <row r="9" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>31.154499999999999</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>79.423699999999997</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>127.559</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>96.273200000000003</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>85.447900000000004</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>165.66200000000001</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>148.26300000000001</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>140.16399999999999</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>155.52099999999999</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <v>232.09</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <v>236.13499999999999</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="5">
         <v>159.11699999999999</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="5">
         <v>216.59899999999999</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="5">
         <v>228.10300000000001</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="5">
         <v>270.19400000000002</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="5">
         <v>266.28300000000002</v>
       </c>
-      <c r="T9" s="6">
+      <c r="T9" s="5">
         <v>268.56900000000002</v>
       </c>
-      <c r="U9" s="6">
+      <c r="U9" s="5">
         <v>333.23</v>
       </c>
-      <c r="V9" s="6">
+      <c r="V9" s="5">
         <v>340.43400000000003</v>
       </c>
-      <c r="W9" s="7">
+      <c r="W9" s="6">
         <v>406.15300000000002</v>
       </c>
     </row>
     <row r="10" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="14">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13">
         <f t="shared" ref="E10:W10" si="37">(E9-D9)/D9</f>
         <v>1.5493492111893947</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <f t="shared" si="37"/>
         <v>0.60605713407962614</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <f t="shared" si="37"/>
         <v>-0.24526532820106769</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <f t="shared" si="37"/>
         <v>-0.11244354607512785</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="13">
         <f t="shared" si="37"/>
         <v>0.93874864098474042</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <f t="shared" si="37"/>
         <v>-0.10502710337916964</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="13">
         <f t="shared" si="37"/>
         <v>-5.4625901270040522E-2</v>
       </c>
-      <c r="L10" s="14">
+      <c r="L10" s="13">
         <f t="shared" si="37"/>
         <v>0.10956451014525842</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="13">
         <f t="shared" si="37"/>
         <v>0.49233865522984049</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="13">
         <f t="shared" si="37"/>
         <v>1.7428583739066687E-2</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10" s="13">
         <f t="shared" si="37"/>
         <v>-0.32616088254600123</v>
       </c>
-      <c r="P10" s="14">
+      <c r="P10" s="13">
         <f t="shared" si="37"/>
         <v>0.36125618255748915</v>
       </c>
-      <c r="Q10" s="14">
+      <c r="Q10" s="13">
         <f t="shared" si="37"/>
         <v>5.3111971892760443E-2</v>
       </c>
-      <c r="R10" s="14">
+      <c r="R10" s="13">
         <f t="shared" si="37"/>
         <v>0.18452628856262304</v>
       </c>
-      <c r="S10" s="14">
+      <c r="S10" s="13">
         <f t="shared" si="37"/>
         <v>-1.4474784784266123E-2</v>
       </c>
-      <c r="T10" s="14">
+      <c r="T10" s="13">
         <f t="shared" si="37"/>
         <v>8.5848514550309306E-3</v>
       </c>
-      <c r="U10" s="14">
+      <c r="U10" s="13">
         <f t="shared" si="37"/>
         <v>0.24076121964932662</v>
       </c>
-      <c r="V10" s="14">
+      <c r="V10" s="13">
         <f t="shared" si="37"/>
         <v>2.1618701797557264E-2</v>
       </c>
-      <c r="W10" s="15">
+      <c r="W10" s="14">
         <f t="shared" si="37"/>
         <v>0.19304476051158223</v>
       </c>
     </row>
     <row r="12" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="6"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
     </row>
     <row r="13" spans="2:24" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>